<commit_message>
Some title abstract screening items
</commit_message>
<xml_diff>
--- a/screening/screening_articles_done.xlsx
+++ b/screening/screening_articles_done.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoffmanka/Documents/dev/smart-on-fhir-literature-research/smart-on-fhir-literature-analysis/screening/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0BEF61-69D3-4E48-B0C2-B8EA3E6B960B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F5C0F-DFDC-B447-93F8-A77BDE12B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="500" windowWidth="48640" windowHeight="29120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="2526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4206" uniqueCount="2528">
   <si>
     <t>id</t>
   </si>
@@ -7601,6 +7601,12 @@
   </si>
   <si>
     <t>usage of SMART</t>
+  </si>
+  <si>
+    <t>no implementation based on SMART, only mentioned in Discussion</t>
+  </si>
+  <si>
+    <t>focus on modeling, no SMART on FHIR</t>
   </si>
 </sst>
 </file>
@@ -8003,8 +8009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U402"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView tabSelected="1" topLeftCell="B342" workbookViewId="0">
+      <selection activeCell="S377" sqref="S377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9211,7 +9217,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>2520</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -9533,8 +9539,14 @@
       <c r="Q32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>204</v>
       </c>
@@ -9574,8 +9586,14 @@
       <c r="P33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
+      <c r="S33" s="3" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>205</v>
       </c>
@@ -9618,8 +9636,14 @@
       <c r="Q34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R34" s="3">
+        <v>0</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>206</v>
       </c>
@@ -9656,8 +9680,14 @@
       <c r="P35" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R35" s="3">
+        <v>0</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>207</v>
       </c>
@@ -9697,8 +9727,14 @@
       <c r="Q36" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R36" s="3">
+        <v>0</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>208</v>
       </c>
@@ -9741,8 +9777,11 @@
       <c r="Q37" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>209</v>
       </c>
@@ -9786,7 +9825,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>210</v>
       </c>
@@ -9827,7 +9866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>211</v>
       </c>
@@ -9868,7 +9907,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>212</v>
       </c>
@@ -9906,7 +9945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>213</v>
       </c>
@@ -9950,7 +9989,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>214</v>
       </c>
@@ -9994,7 +10033,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>215</v>
       </c>
@@ -10038,7 +10077,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>216</v>
       </c>
@@ -10079,7 +10118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>217</v>
       </c>
@@ -10120,7 +10159,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>218</v>
       </c>
@@ -10158,7 +10197,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>219</v>
       </c>
@@ -18958,7 +18997,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>428</v>
       </c>
@@ -18999,7 +19038,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>429</v>
       </c>
@@ -19043,7 +19082,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>430</v>
       </c>
@@ -19084,7 +19123,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>431</v>
       </c>
@@ -19128,7 +19167,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>432</v>
       </c>
@@ -19172,7 +19211,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>433</v>
       </c>
@@ -19210,7 +19249,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>434</v>
       </c>
@@ -19254,7 +19293,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>435</v>
       </c>
@@ -19295,7 +19334,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>436</v>
       </c>
@@ -19336,7 +19375,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>437</v>
       </c>
@@ -19379,8 +19418,11 @@
       <c r="Q266" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R266" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>438</v>
       </c>
@@ -19424,7 +19466,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>439</v>
       </c>
@@ -19465,7 +19507,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>440</v>
       </c>
@@ -19503,7 +19545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>441</v>
       </c>
@@ -19546,8 +19588,11 @@
       <c r="Q270" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R270" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>442</v>
       </c>
@@ -19590,8 +19635,14 @@
       <c r="Q271" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R271" s="3">
+        <v>0</v>
+      </c>
+      <c r="S271" s="3" t="s">
+        <v>2523</v>
+      </c>
+    </row>
+    <row r="272" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>443</v>
       </c>
@@ -19634,8 +19685,14 @@
       <c r="Q272" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R272" s="3">
+        <v>0</v>
+      </c>
+      <c r="S272" s="3" t="s">
+        <v>2523</v>
+      </c>
+    </row>
+    <row r="273" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>444</v>
       </c>
@@ -19678,8 +19735,14 @@
       <c r="Q273" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R273" s="3">
+        <v>0</v>
+      </c>
+      <c r="S273" s="3" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="274" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>445</v>
       </c>
@@ -19722,8 +19785,11 @@
       <c r="Q274" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R274" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>446</v>
       </c>
@@ -19767,7 +19833,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>447</v>
       </c>
@@ -19811,7 +19877,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="277" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>448</v>
       </c>
@@ -19855,7 +19921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>449</v>
       </c>
@@ -19899,7 +19965,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>450</v>
       </c>
@@ -19943,7 +20009,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>451</v>
       </c>
@@ -19987,7 +20053,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="281" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>452</v>
       </c>
@@ -20034,7 +20100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>453</v>
       </c>
@@ -20078,7 +20144,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>454</v>
       </c>
@@ -20122,7 +20188,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="284" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>455</v>
       </c>
@@ -20163,7 +20229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="285" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>456</v>
       </c>
@@ -20204,7 +20270,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="286" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>457</v>
       </c>
@@ -20245,7 +20311,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="287" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>458</v>
       </c>
@@ -20289,7 +20355,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="288" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>459</v>
       </c>
@@ -24115,6 +24181,9 @@
       </c>
       <c r="Q377" t="s">
         <v>39</v>
+      </c>
+      <c r="R377" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:19" x14ac:dyDescent="0.2">

</xml_diff>